<commit_message>
cleaning up repo and updating supplement
</commit_message>
<xml_diff>
--- a/results/tables/table_S2.xlsx
+++ b/results/tables/table_S2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="114">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -373,6 +373,18 @@
   </si>
   <si>
     <t xml:space="preserve">Pi exchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transcript abundance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low confidence: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">High confidence:</t>
   </si>
 </sst>
 </file>
@@ -496,7 +508,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -553,6 +565,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1510,18 +1530,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.52"/>
@@ -1749,6 +1769,50 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>